<commit_message>
fix 1620 point values in grading scale
</commit_message>
<xml_diff>
--- a/BIOL1620/1620_sheets.xlsx
+++ b/BIOL1620/1620_sheets.xlsx
@@ -95,7 +95,7 @@
     <t xml:space="preserve">E</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;480</t>
+    <t xml:space="preserve">&lt;380</t>
   </si>
 </sst>
 </file>
@@ -110,6 +110,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -180,18 +181,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -201,11 +202,10 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -286,21 +286,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,7 +314,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>700</v>
+        <v>600</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,7 +322,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>690</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,7 +330,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>640</v>
+        <v>540</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,7 +338,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>630</v>
+        <v>530</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,7 +346,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>560</v>
+        <v>460</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,7 +354,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>550</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +362,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>480</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,7 +376,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>